<commit_message>
All initial necessary info written
Still under development, however it is ready to be used as a foundation for creating the game. Many different game aspects have hopefully been segregated into concise systems to make development easier.
</commit_message>
<xml_diff>
--- a/Mechanics for BlenderMan.xlsx
+++ b/Mechanics for BlenderMan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eltim\OneDrive\Documents\Excel Documents\Game Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF76FFF6-6CBC-48A7-A8DD-5DC8A734A859}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92AB91C-148F-4DD7-8ECD-DEB5BF30F6C0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12585" yWindow="4590" windowWidth="17505" windowHeight="10605" xr2:uid="{A287A8CC-055B-4F44-890F-7807B9B4EDB6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{A287A8CC-055B-4F44-890F-7807B9B4EDB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="91">
   <si>
     <t>ACTION</t>
   </si>
@@ -39,9 +39,6 @@
     <t>PURPOSE</t>
   </si>
   <si>
-    <t>SYSTEM</t>
-  </si>
-  <si>
     <t>CHALLENGE</t>
   </si>
   <si>
@@ -57,9 +54,6 @@
     <t>Level Traversal</t>
   </si>
   <si>
-    <t>Movement</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -87,9 +81,6 @@
     <t>Sprinting</t>
   </si>
   <si>
-    <t>Movement Ability</t>
-  </si>
-  <si>
     <t>Power-Up</t>
   </si>
   <si>
@@ -108,9 +99,6 @@
     <t>Level Traversal/Combat</t>
   </si>
   <si>
-    <t>Movement/Combat</t>
-  </si>
-  <si>
     <t>Traversal</t>
   </si>
   <si>
@@ -201,36 +189,12 @@
     <t>Varied/Animation</t>
   </si>
   <si>
-    <t>Buy/Sell</t>
-  </si>
-  <si>
-    <t>Shops/End of Levels</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>Currency</t>
-  </si>
-  <si>
-    <t>Reource Aquirement</t>
-  </si>
-  <si>
     <t>Aiming(Standing)</t>
   </si>
   <si>
     <t>Double Jump</t>
   </si>
   <si>
-    <t>Combat Ability</t>
-  </si>
-  <si>
-    <t>Resource Gathering Ability</t>
-  </si>
-  <si>
-    <t>Level Traversal/Combat Ability</t>
-  </si>
-  <si>
     <t>TRIGGER (When does game prompt for use)</t>
   </si>
   <si>
@@ -241,6 +205,105 @@
   </si>
   <si>
     <t>LIMITATIONS</t>
+  </si>
+  <si>
+    <t>CONTROLS (keys)</t>
+  </si>
+  <si>
+    <t>Walk Left - A; Walk Right - D</t>
+  </si>
+  <si>
+    <t>Hold Shift Key whilst pressing A./D</t>
+  </si>
+  <si>
+    <t>Suction - Down Arrow</t>
+  </si>
+  <si>
+    <t>Suction - Down Arrow whilst walking</t>
+  </si>
+  <si>
+    <t>Blend - Up Arrow</t>
+  </si>
+  <si>
+    <t>Up arrow whilst walking</t>
+  </si>
+  <si>
+    <t>Interact</t>
+  </si>
+  <si>
+    <t>Shops/NPCs</t>
+  </si>
+  <si>
+    <t>Interact - E</t>
+  </si>
+  <si>
+    <t>Change Blending Mode - Right Arrow</t>
+  </si>
+  <si>
+    <t>Change Power-Up - Left Arrow</t>
+  </si>
+  <si>
+    <t>Sprint -  (Use Powerup) A/D</t>
+  </si>
+  <si>
+    <t>Pause Game - ESC</t>
+  </si>
+  <si>
+    <t>Menu Confirmation - Enter</t>
+  </si>
+  <si>
+    <t>Menu Selection - W/S</t>
+  </si>
+  <si>
+    <t>Jump - Space Bar</t>
+  </si>
+  <si>
+    <t>Blast/Heal - W</t>
+  </si>
+  <si>
+    <t>W whilst walking</t>
+  </si>
+  <si>
+    <t>W whilst running</t>
+  </si>
+  <si>
+    <t>Use Power-Ups - Q</t>
+  </si>
+  <si>
+    <t>Double Jump - Press Space Bar while in air</t>
+  </si>
+  <si>
+    <t>Empty Container - T</t>
+  </si>
+  <si>
+    <t>Progression</t>
+  </si>
+  <si>
+    <t>Economy</t>
+  </si>
+  <si>
+    <t>SYSTEM (All of these are implicitly assigned to the Animation System)</t>
+  </si>
+  <si>
+    <t>Game World</t>
+  </si>
+  <si>
+    <t>Inventory</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Progression</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>Spin Attack - S</t>
+  </si>
+  <si>
+    <t>Float - F</t>
+  </si>
+  <si>
+    <t>Aim - C along with Arrow Keys</t>
   </si>
 </sst>
 </file>
@@ -290,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -302,6 +365,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0407D8EA-A6D2-4FC8-B5AE-E6FF22D1D1CB}">
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,9 +695,10 @@
     <col min="7" max="8" width="18.28515625" customWidth="1"/>
     <col min="9" max="9" width="18.140625" customWidth="1"/>
     <col min="10" max="10" width="18.85546875" customWidth="1"/>
+    <col min="11" max="11" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -641,575 +706,629 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="K16" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="G18" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="I18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J18" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1221,7 +1340,7 @@
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1232,8 +1351,11 @@
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1244,8 +1366,11 @@
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1256,8 +1381,11 @@
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1268,8 +1396,11 @@
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1280,8 +1411,11 @@
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1292,8 +1426,11 @@
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1305,7 +1442,7 @@
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1317,7 +1454,7 @@
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1329,7 +1466,7 @@
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1341,7 +1478,7 @@
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1353,7 +1490,7 @@
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1365,7 +1502,7 @@
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>

</xml_diff>